<commit_message>
Incremental bug fixing for monoclinic reindexing.
</commit_message>
<xml_diff>
--- a/data/GroupSpec_monoclinic.xlsx
+++ b/data/GroupSpec_monoclinic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7195D903-DBBE-B140-9829-EBEABAE069BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E153CE64-1DD1-1445-91B5-5044CECDD679}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1460" yWindow="-19540" windowWidth="29500" windowHeight="17000" activeTab="1" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="-2280" yWindow="-18460" windowWidth="29500" windowHeight="17000" activeTab="1" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -4766,8 +4766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA525AC-850D-B244-AB53-A3DA79E8EC77}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Last bug fixes for monoclinic reindexing
</commit_message>
<xml_diff>
--- a/data/GroupSpec_monoclinic.xlsx
+++ b/data/GroupSpec_monoclinic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E153CE64-1DD1-1445-91B5-5044CECDD679}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C8230A-68FA-054A-A810-1CD58E6F4804}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2280" yWindow="-18460" windowWidth="29500" windowHeight="17000" activeTab="1" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="-2280" yWindow="-18460" windowWidth="29500" windowHeight="17000" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -927,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E9EF93-9C26-5E4D-979F-BFF17FE810E6}">
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>4797</v>
+        <v>4799</v>
       </c>
       <c r="K4" t="s">
         <v>146</v>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="F6" t="s">
         <v>155</v>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H12" t="s">
         <v>147</v>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s">
         <v>148</v>
@@ -1528,6 +1528,9 @@
       <c r="C21">
         <v>0</v>
       </c>
+      <c r="E21">
+        <v>2123</v>
+      </c>
       <c r="F21" t="s">
         <v>155</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
         <v>154</v>
@@ -1712,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="K27" t="s">
         <v>146</v>
@@ -1764,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="F29" t="s">
         <v>155</v>
@@ -1796,7 +1799,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
         <v>154</v>
@@ -1828,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" t="s">
         <v>156</v>
@@ -1863,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" t="s">
         <v>157</v>
@@ -1898,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="H33" t="s">
         <v>147</v>
@@ -1918,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H34" t="s">
         <v>148</v>
@@ -1938,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H35" t="s">
         <v>149</v>
@@ -2025,7 +2028,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>4886</v>
+        <v>4893</v>
       </c>
       <c r="H38" t="s">
         <v>147</v>
@@ -2048,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>1783</v>
+        <v>1627</v>
       </c>
       <c r="H39" t="s">
         <v>148</v>
@@ -2071,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>4894</v>
+        <v>4892</v>
       </c>
       <c r="H40" t="s">
         <v>149</v>
@@ -2167,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>4909</v>
+        <v>4912</v>
       </c>
       <c r="F43" t="s">
         <v>155</v>
@@ -2202,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="F44" t="s">
         <v>154</v>
@@ -2237,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F45" t="s">
         <v>156</v>
@@ -2353,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>4853</v>
+        <v>4871</v>
       </c>
       <c r="L49" t="s">
         <v>147</v>
@@ -2370,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F50" t="s">
         <v>155</v>
@@ -2437,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="E52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F52" t="s">
         <v>149</v>
@@ -2584,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I58" t="s">
         <v>146</v>
@@ -2604,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I59" t="s">
         <v>155</v>
@@ -2804,7 +2807,7 @@
         <v>1</v>
       </c>
       <c r="E66">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>154</v>
@@ -2839,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F67" t="s">
         <v>149</v>
@@ -2923,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="E70">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
@@ -2969,7 +2972,7 @@
         <v>1</v>
       </c>
       <c r="E72">
-        <v>3162</v>
+        <v>3156</v>
       </c>
       <c r="L72" t="s">
         <v>147</v>
@@ -3021,7 +3024,7 @@
         <v>1</v>
       </c>
       <c r="E74">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>154</v>
@@ -3054,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="E75">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F75" t="s">
         <v>154</v>
@@ -3135,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="E78">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I78" t="s">
         <v>148</v>
@@ -3155,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="E79">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I79" t="s">
         <v>146</v>
@@ -3262,7 +3265,7 @@
         <v>1</v>
       </c>
       <c r="E83">
-        <v>4883</v>
+        <v>4891</v>
       </c>
       <c r="I83" t="s">
         <v>148</v>
@@ -3285,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="E84">
-        <v>2952</v>
+        <v>2777</v>
       </c>
       <c r="I84" t="s">
         <v>146</v>
@@ -3308,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="E85">
-        <v>4907</v>
+        <v>4901</v>
       </c>
       <c r="I85" t="s">
         <v>155</v>
@@ -3404,7 +3407,7 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>4906</v>
+        <v>4915</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>154</v>
@@ -3439,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F89" t="s">
         <v>149</v>
@@ -3474,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F90" t="s">
         <v>156</v>
@@ -3523,7 +3526,7 @@
         <v>2</v>
       </c>
       <c r="E92">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
@@ -3569,7 +3572,7 @@
         <v>2</v>
       </c>
       <c r="E94">
-        <v>4808</v>
+        <v>4813</v>
       </c>
       <c r="J94" t="s">
         <v>148</v>
@@ -3621,7 +3624,7 @@
         <v>2</v>
       </c>
       <c r="E96">
-        <v>4862</v>
+        <v>4854</v>
       </c>
       <c r="F96" t="s">
         <v>149</v>
@@ -3653,7 +3656,7 @@
         <v>2</v>
       </c>
       <c r="E97">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F97" t="s">
         <v>155</v>
@@ -3734,7 +3737,7 @@
         <v>2</v>
       </c>
       <c r="E100">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.2">
@@ -3780,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="E102">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="G102" t="s">
         <v>146</v>
@@ -3800,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="E103">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G103" t="s">
         <v>147</v>
@@ -3820,7 +3823,7 @@
         <v>2</v>
       </c>
       <c r="E104">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G104" t="s">
         <v>154</v>
@@ -4055,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="E112">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F112" t="s">
         <v>155</v>
@@ -4139,7 +4142,7 @@
         <v>2</v>
       </c>
       <c r="E115">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
@@ -4185,7 +4188,7 @@
         <v>2</v>
       </c>
       <c r="E117">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="J117" t="s">
         <v>148</v>
@@ -4237,7 +4240,7 @@
         <v>2</v>
       </c>
       <c r="E119">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="F119" t="s">
         <v>149</v>
@@ -4269,7 +4272,7 @@
         <v>2</v>
       </c>
       <c r="E120">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F120" t="s">
         <v>155</v>
@@ -4301,7 +4304,7 @@
         <v>2</v>
       </c>
       <c r="E121">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F121" t="s">
         <v>156</v>
@@ -4350,7 +4353,7 @@
         <v>2</v>
       </c>
       <c r="E123">
-        <v>2877</v>
+        <v>2871</v>
       </c>
       <c r="G123" t="s">
         <v>146</v>
@@ -4370,7 +4373,7 @@
         <v>2</v>
       </c>
       <c r="E124">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="G124" t="s">
         <v>147</v>
@@ -4390,7 +4393,7 @@
         <v>2</v>
       </c>
       <c r="E125">
-        <v>1993</v>
+        <v>1985</v>
       </c>
       <c r="G125" t="s">
         <v>154</v>
@@ -4477,7 +4480,7 @@
         <v>2</v>
       </c>
       <c r="E128">
-        <v>4866</v>
+        <v>4895</v>
       </c>
       <c r="G128" t="s">
         <v>146</v>
@@ -4500,7 +4503,7 @@
         <v>2</v>
       </c>
       <c r="E129">
-        <v>3526</v>
+        <v>3346</v>
       </c>
       <c r="G129" t="s">
         <v>147</v>
@@ -4619,7 +4622,7 @@
         <v>2</v>
       </c>
       <c r="E133">
-        <v>4916</v>
+        <v>4911</v>
       </c>
       <c r="F133" t="s">
         <v>149</v>
@@ -4654,7 +4657,7 @@
         <v>2</v>
       </c>
       <c r="E134">
-        <v>226</v>
+        <v>128</v>
       </c>
       <c r="F134" t="s">
         <v>155</v>
@@ -4689,7 +4692,7 @@
         <v>2</v>
       </c>
       <c r="E135">
-        <v>2942</v>
+        <v>2934</v>
       </c>
       <c r="F135" t="s">
         <v>156</v>
@@ -4766,8 +4769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA525AC-850D-B244-AB53-A3DA79E8EC77}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5367,6 +5370,9 @@
       <c r="D27" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="E27">
+        <v>2123</v>
+      </c>
       <c r="F27" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Changed monoclinic reindexing to reindex to common settings.
</commit_message>
<xml_diff>
--- a/data/GroupSpec_monoclinic.xlsx
+++ b/data/GroupSpec_monoclinic.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67838449-D711-524E-BB9F-7AA3A4B732D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A0E225-4A62-7B44-9E37-24A01468CF8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2280" yWindow="-18460" windowWidth="29500" windowHeight="17000" activeTab="2" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="400" yWindow="1560" windowWidth="29500" windowHeight="17000" activeTab="3" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V0" sheetId="2" r:id="rId2"/>
     <sheet name="Groups V1" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups V2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="200">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -594,6 +595,39 @@
   </si>
   <si>
     <t>monoclinic_2_07</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>acb</t>
+  </si>
+  <si>
+    <t>cab</t>
+  </si>
+  <si>
+    <t>cba</t>
+  </si>
+  <si>
+    <t>bac</t>
+  </si>
+  <si>
+    <t>bca</t>
+  </si>
+  <si>
+    <t>monoclinic_00</t>
+  </si>
+  <si>
+    <t>monoclinic_01</t>
+  </si>
+  <si>
+    <t>monoclinic_02</t>
+  </si>
+  <si>
+    <t>monoclinic_03</t>
+  </si>
+  <si>
+    <t>total counts</t>
   </si>
 </sst>
 </file>
@@ -956,7 +990,7 @@
   <dimension ref="A1:L168"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7462,8 +7496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DFFAFD-7483-144A-957A-73E2CBBDDA77}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10136,4 +10170,849 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB10BC37-39A0-404D-8981-2DDCADDC0F1B}">
+  <dimension ref="A1:R63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J1" t="s">
+        <v>193</v>
+      </c>
+      <c r="K1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2">
+        <v>140</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>102</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>21</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4">
+        <v>183</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>97</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5">
+        <v>24186</v>
+      </c>
+      <c r="F5">
+        <v>5948</v>
+      </c>
+      <c r="G5">
+        <v>10321</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>7914</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6">
+        <v>4553</v>
+      </c>
+      <c r="F6">
+        <v>824</v>
+      </c>
+      <c r="G6">
+        <v>2795</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>934</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f>SUM(F2:F6)</f>
+        <v>6850</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:K7" si="0">SUM(G2:G6)</f>
+        <v>13192</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>9068</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9">
+        <f>SUM(F9:K9)</f>
+        <v>2925</v>
+      </c>
+      <c r="F9">
+        <v>530</v>
+      </c>
+      <c r="G9">
+        <v>611</v>
+      </c>
+      <c r="H9">
+        <v>132</v>
+      </c>
+      <c r="I9">
+        <v>79</v>
+      </c>
+      <c r="J9">
+        <v>1376</v>
+      </c>
+      <c r="K9">
+        <v>197</v>
+      </c>
+      <c r="N9" t="s">
+        <v>147</v>
+      </c>
+      <c r="R9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:E11" si="1">SUM(F10:K10)</f>
+        <v>4856</v>
+      </c>
+      <c r="F10">
+        <v>558</v>
+      </c>
+      <c r="G10">
+        <v>209</v>
+      </c>
+      <c r="H10">
+        <v>91</v>
+      </c>
+      <c r="I10">
+        <v>87</v>
+      </c>
+      <c r="J10">
+        <v>3259</v>
+      </c>
+      <c r="K10">
+        <v>652</v>
+      </c>
+      <c r="N10" t="s">
+        <v>147</v>
+      </c>
+      <c r="R10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>179758</v>
+      </c>
+      <c r="F11">
+        <v>32572</v>
+      </c>
+      <c r="G11">
+        <v>48752</v>
+      </c>
+      <c r="H11">
+        <v>11287</v>
+      </c>
+      <c r="I11">
+        <v>4655</v>
+      </c>
+      <c r="J11">
+        <v>69688</v>
+      </c>
+      <c r="K11">
+        <v>12804</v>
+      </c>
+      <c r="N11" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>146</v>
+      </c>
+      <c r="R11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f>SUM(F9:F11)</f>
+        <v>33660</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:K12" si="2">SUM(G9:G11)</f>
+        <v>49572</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>11510</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>4821</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>74323</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>13653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E16" si="3">SUM(F14:K14)</f>
+        <v>469</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>43</v>
+      </c>
+      <c r="H14">
+        <v>255</v>
+      </c>
+      <c r="I14">
+        <v>104</v>
+      </c>
+      <c r="J14">
+        <v>16</v>
+      </c>
+      <c r="K14">
+        <v>46</v>
+      </c>
+      <c r="L14" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" t="s">
+        <v>146</v>
+      </c>
+      <c r="N14" t="s">
+        <v>148</v>
+      </c>
+      <c r="O14" t="s">
+        <v>155</v>
+      </c>
+      <c r="P14" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>6542</v>
+      </c>
+      <c r="F15">
+        <v>220</v>
+      </c>
+      <c r="G15">
+        <v>373</v>
+      </c>
+      <c r="H15">
+        <v>1695</v>
+      </c>
+      <c r="I15">
+        <v>1775</v>
+      </c>
+      <c r="J15">
+        <v>393</v>
+      </c>
+      <c r="K15">
+        <v>2086</v>
+      </c>
+      <c r="L15" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" t="s">
+        <v>146</v>
+      </c>
+      <c r="N15" t="s">
+        <v>148</v>
+      </c>
+      <c r="O15" t="s">
+        <v>155</v>
+      </c>
+      <c r="P15" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>6137</v>
+      </c>
+      <c r="F16">
+        <v>150</v>
+      </c>
+      <c r="G16">
+        <v>90</v>
+      </c>
+      <c r="H16">
+        <v>329</v>
+      </c>
+      <c r="I16">
+        <v>973</v>
+      </c>
+      <c r="J16">
+        <v>905</v>
+      </c>
+      <c r="K16">
+        <v>3690</v>
+      </c>
+      <c r="L16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M16" t="s">
+        <v>146</v>
+      </c>
+      <c r="N16" t="s">
+        <v>148</v>
+      </c>
+      <c r="O16" t="s">
+        <v>155</v>
+      </c>
+      <c r="P16" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f>SUM(F14:F16)</f>
+        <v>375</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17" si="4">SUM(G14:G16)</f>
+        <v>506</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17" si="5">SUM(H14:H16)</f>
+        <v>2279</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17" si="6">SUM(I14:I16)</f>
+        <v>2852</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17" si="7">SUM(J14:J16)</f>
+        <v>1314</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17" si="8">SUM(K14:K16)</f>
+        <v>5822</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E20" si="9">SUM(F19:K19)</f>
+        <v>8337</v>
+      </c>
+      <c r="F19">
+        <v>960</v>
+      </c>
+      <c r="G19">
+        <v>1700</v>
+      </c>
+      <c r="H19">
+        <v>1494</v>
+      </c>
+      <c r="I19">
+        <v>933</v>
+      </c>
+      <c r="J19">
+        <v>1123</v>
+      </c>
+      <c r="K19">
+        <v>2127</v>
+      </c>
+      <c r="L19" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" t="s">
+        <v>146</v>
+      </c>
+      <c r="N19" t="s">
+        <v>150</v>
+      </c>
+      <c r="O19" t="s">
+        <v>155</v>
+      </c>
+      <c r="P19" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>146</v>
+      </c>
+      <c r="R19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="9"/>
+        <v>64833</v>
+      </c>
+      <c r="F20">
+        <v>3967</v>
+      </c>
+      <c r="G20">
+        <v>3252</v>
+      </c>
+      <c r="H20">
+        <v>4181</v>
+      </c>
+      <c r="I20">
+        <v>7632</v>
+      </c>
+      <c r="J20">
+        <v>13112</v>
+      </c>
+      <c r="K20">
+        <v>32689</v>
+      </c>
+      <c r="L20" t="s">
+        <v>155</v>
+      </c>
+      <c r="M20" t="s">
+        <v>146</v>
+      </c>
+      <c r="N20" t="s">
+        <v>150</v>
+      </c>
+      <c r="O20" t="s">
+        <v>155</v>
+      </c>
+      <c r="P20" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>146</v>
+      </c>
+      <c r="R20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>SUM(F19:F20)</f>
+        <v>4927</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:K21" si="10">SUM(G19:G20)</f>
+        <v>4952</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="10"/>
+        <v>5675</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="10"/>
+        <v>8565</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="10"/>
+        <v>14235</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="10"/>
+        <v>34816</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored codebase to do optimization based on Bravais lattice and implemented a generalized templating approach
</commit_message>
<xml_diff>
--- a/data/GroupSpec_monoclinic.xlsx
+++ b/data/GroupSpec_monoclinic.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A0E225-4A62-7B44-9E37-24A01468CF8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BD94E7-AA58-8543-9A10-AD9D0D02EBE8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="1560" windowWidth="29500" windowHeight="17000" activeTab="3" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="3280" yWindow="-18380" windowWidth="22980" windowHeight="17000" activeTab="4" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V0" sheetId="2" r:id="rId2"/>
     <sheet name="Groups V1" sheetId="3" r:id="rId3"/>
     <sheet name="Groups V2" sheetId="4" r:id="rId4"/>
+    <sheet name="groups_v3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="201">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -628,6 +629,9 @@
   </si>
   <si>
     <t>total counts</t>
+  </si>
+  <si>
+    <t>h + l = 2n; h, l = 2n</t>
   </si>
 </sst>
 </file>
@@ -7496,7 +7500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DFFAFD-7483-144A-957A-73E2CBBDDA77}">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -10176,8 +10180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB10BC37-39A0-404D-8981-2DDCADDC0F1B}">
   <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11015,4 +11019,599 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9406A21-5309-FB4C-9C4E-9E8239DEBBF3}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2">
+        <f>SUM(F2:H2)</f>
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>89</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3">
+        <f>SUM(F3:H3)</f>
+        <v>46</v>
+      </c>
+      <c r="F3">
+        <v>18</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E4">
+        <f>SUM(F4:H4)</f>
+        <v>161</v>
+      </c>
+      <c r="F4">
+        <v>89</v>
+      </c>
+      <c r="G4">
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E5">
+        <f>SUM(F5:H5)</f>
+        <v>23499</v>
+      </c>
+      <c r="F5">
+        <v>7664</v>
+      </c>
+      <c r="G5">
+        <v>5752</v>
+      </c>
+      <c r="H5">
+        <v>10083</v>
+      </c>
+      <c r="N5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6">
+        <f>SUM(F6:H6)</f>
+        <v>4435</v>
+      </c>
+      <c r="F6">
+        <v>916</v>
+      </c>
+      <c r="G6">
+        <v>794</v>
+      </c>
+      <c r="H6">
+        <v>2725</v>
+      </c>
+      <c r="N6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f>SUM(F2:F6)</f>
+        <v>8776</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ref="G7:H7" si="0">SUM(G2:G6)</f>
+        <v>6613</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>12872</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9">
+        <f>SUM(F9:H9)</f>
+        <v>2866</v>
+      </c>
+      <c r="F9">
+        <v>1207</v>
+      </c>
+      <c r="G9">
+        <v>909</v>
+      </c>
+      <c r="H9">
+        <v>750</v>
+      </c>
+      <c r="K9" t="s">
+        <v>147</v>
+      </c>
+      <c r="O9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
+      </c>
+      <c r="E10">
+        <f>SUM(F10:H10)</f>
+        <v>4875</v>
+      </c>
+      <c r="F10">
+        <v>3588</v>
+      </c>
+      <c r="G10">
+        <v>930</v>
+      </c>
+      <c r="H10">
+        <v>357</v>
+      </c>
+      <c r="K10" t="s">
+        <v>147</v>
+      </c>
+      <c r="O10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11">
+        <f>SUM(F11:H11)</f>
+        <v>29342</v>
+      </c>
+      <c r="F11">
+        <v>10407</v>
+      </c>
+      <c r="G11">
+        <v>8900</v>
+      </c>
+      <c r="H11">
+        <v>10035</v>
+      </c>
+      <c r="K11" t="s">
+        <v>147</v>
+      </c>
+      <c r="N11" t="s">
+        <v>146</v>
+      </c>
+      <c r="O11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <f>SUM(F9:F11)</f>
+        <v>15202</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12" si="1">SUM(G9:G11)</f>
+        <v>10739</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ref="H12" si="2">SUM(H9:H11)</f>
+        <v>11142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14">
+        <f>SUM(F14:H14)</f>
+        <v>450</v>
+      </c>
+      <c r="F14">
+        <v>60</v>
+      </c>
+      <c r="G14">
+        <v>85</v>
+      </c>
+      <c r="H14">
+        <v>305</v>
+      </c>
+      <c r="I14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J14" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" t="s">
+        <v>149</v>
+      </c>
+      <c r="L14" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" t="s">
+        <v>148</v>
+      </c>
+      <c r="N14" t="s">
+        <v>146</v>
+      </c>
+      <c r="O14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15">
+        <f>SUM(F15:H15)</f>
+        <v>6376</v>
+      </c>
+      <c r="F15">
+        <v>2608</v>
+      </c>
+      <c r="G15">
+        <v>1760</v>
+      </c>
+      <c r="H15">
+        <v>2008</v>
+      </c>
+      <c r="I15" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" t="s">
+        <v>149</v>
+      </c>
+      <c r="L15" t="s">
+        <v>155</v>
+      </c>
+      <c r="M15" t="s">
+        <v>148</v>
+      </c>
+      <c r="N15" t="s">
+        <v>146</v>
+      </c>
+      <c r="O15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16">
+        <f>SUM(F16:H16)</f>
+        <v>5968</v>
+      </c>
+      <c r="F16">
+        <v>4614</v>
+      </c>
+      <c r="G16">
+        <v>951</v>
+      </c>
+      <c r="H16">
+        <v>403</v>
+      </c>
+      <c r="I16" t="s">
+        <v>156</v>
+      </c>
+      <c r="J16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" t="s">
+        <v>149</v>
+      </c>
+      <c r="L16" t="s">
+        <v>155</v>
+      </c>
+      <c r="M16" t="s">
+        <v>148</v>
+      </c>
+      <c r="N16" t="s">
+        <v>146</v>
+      </c>
+      <c r="O16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f>SUM(F14:F16)</f>
+        <v>7282</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17:H17" si="3">SUM(G14:G16)</f>
+        <v>2796</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>2716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E19">
+        <f>SUM(F19:H19)</f>
+        <v>8180</v>
+      </c>
+      <c r="F19">
+        <v>4109</v>
+      </c>
+      <c r="G19">
+        <v>1269</v>
+      </c>
+      <c r="H19">
+        <v>2802</v>
+      </c>
+      <c r="I19" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" t="s">
+        <v>154</v>
+      </c>
+      <c r="K19" t="s">
+        <v>200</v>
+      </c>
+      <c r="L19" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" t="s">
+        <v>148</v>
+      </c>
+      <c r="N19" t="s">
+        <v>146</v>
+      </c>
+      <c r="O19" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E20">
+        <f>SUM(F20:H20)</f>
+        <v>29512</v>
+      </c>
+      <c r="F20">
+        <v>22748</v>
+      </c>
+      <c r="G20">
+        <v>3890</v>
+      </c>
+      <c r="H20">
+        <v>2874</v>
+      </c>
+      <c r="I20" t="s">
+        <v>156</v>
+      </c>
+      <c r="J20" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" t="s">
+        <v>200</v>
+      </c>
+      <c r="L20" t="s">
+        <v>155</v>
+      </c>
+      <c r="M20" t="s">
+        <v>148</v>
+      </c>
+      <c r="N20" t="s">
+        <v>146</v>
+      </c>
+      <c r="O20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>SUM(F19:F20)</f>
+        <v>26857</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:H21" si="4">SUM(G19:G20)</f>
+        <v>5159</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>5676</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Diagnostic plots added to Optimization
</commit_message>
<xml_diff>
--- a/data/GroupSpec_monoclinic.xlsx
+++ b/data/GroupSpec_monoclinic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36797C9-87D0-3446-9A9B-8F14BD9A3ECB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92522DAD-A37B-A64C-BA15-2C44E1363BB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="-18380" windowWidth="22980" windowHeight="17000" activeTab="4" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="2000" yWindow="1780" windowWidth="22980" windowHeight="17000" activeTab="4" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="201">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -11025,13 +11025,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9406A21-5309-FB4C-9C4E-9E8239DEBBF3}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -11254,7 +11256,10 @@
         <v>750</v>
       </c>
       <c r="K9" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="M9" t="s">
+        <v>148</v>
       </c>
       <c r="O9" t="s">
         <v>147</v>
@@ -11287,7 +11292,10 @@
         <v>357</v>
       </c>
       <c r="K10" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="M10" t="s">
+        <v>148</v>
       </c>
       <c r="O10" t="s">
         <v>147</v>
@@ -11320,7 +11328,10 @@
         <v>10035</v>
       </c>
       <c r="K11" t="s">
-        <v>147</v>
+        <v>149</v>
+      </c>
+      <c r="M11" t="s">
+        <v>148</v>
       </c>
       <c r="N11" t="s">
         <v>146</v>

</xml_diff>